<commit_message>
IAE 1 - 26/08/2025
</commit_message>
<xml_diff>
--- a/SEM 5/Progress.xlsx
+++ b/SEM 5/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Degree\SEM 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A5520E-4026-41EC-9D99-067ADD5ED5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693F12E4-63E6-4EA4-B4A8-B3A45BF54978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,9 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -550,7 +553,7 @@
   <dimension ref="B2:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,8 +696,8 @@
       <c r="G7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>37</v>
+      <c r="H7" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>37</v>
@@ -713,8 +716,8 @@
       <c r="D8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>37</v>
+      <c r="E8" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>37</v>
@@ -722,8 +725,8 @@
       <c r="G8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>37</v>
+      <c r="H8" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>37</v>
@@ -736,14 +739,14 @@
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>37</v>
+      <c r="C9" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>37</v>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
IA 2 - 16/10/2025
</commit_message>
<xml_diff>
--- a/SEM 5/Progress.xlsx
+++ b/SEM 5/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Degree\SEM 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102F11BC-ED6F-46EC-92FB-A23C00BBBAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E432B46-419E-46B7-BFAF-B7E60491748E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="B2:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,8 +912,8 @@
       <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>27</v>
+      <c r="C16" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>16</v>
@@ -941,8 +941,8 @@
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>27</v>
+      <c r="C17" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>16</v>
@@ -1017,8 +1017,8 @@
       <c r="G20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>27</v>
+      <c r="H20" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>16</v>
@@ -1046,8 +1046,8 @@
       <c r="G21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>27</v>
+      <c r="H21" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>16</v>

</xml_diff>